<commit_message>
Making default file extension type of MDL files ".xml" rather than ".mdl". Replaced the example MDL file with the one of the same name but with the file extension ".xml" rather than ".mdl" README updated with the updated file extension for the sample files.
</commit_message>
<xml_diff>
--- a/Scenarios/FlightTesting/Utilities/TxOpScheduleViewer/MDL_Shell_Generator/BRASS-Example_Flight_Test_Schedule.xlsx
+++ b/Scenarios/FlightTesting/Utilities/TxOpScheduleViewer/MDL_Shell_Generator/BRASS-Example_Flight_Test_Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tnewton/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tnewton/PycharmProjects/challenge-problems/Scenarios/FlightTesting/Utilities/TxOpScheduleViewer/MDL_Shell_Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC33FE01-2FA7-0D40-9EC0-05F43E6DB8FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01FF474-41A9-0D44-94F9-52C6F42BDC0F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38020" yWindow="-2160" windowWidth="33080" windowHeight="21660" xr2:uid="{7BA411C7-B93B-8342-BCD4-9C4A4FD828FC}"/>
   </bookViews>
@@ -583,10 +583,10 @@
   <dimension ref="A1:U162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="12" topLeftCell="C108" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B57" sqref="A57:XFD57"/>
+      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3626,13 +3626,12 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A157:A162"/>
-    <mergeCell ref="A121:A126"/>
-    <mergeCell ref="A127:A132"/>
-    <mergeCell ref="A133:A138"/>
-    <mergeCell ref="A139:A144"/>
-    <mergeCell ref="A145:A150"/>
-    <mergeCell ref="A151:A156"/>
+    <mergeCell ref="A43:A48"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A25:A30"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="A37:A42"/>
     <mergeCell ref="A115:A120"/>
     <mergeCell ref="A49:A54"/>
     <mergeCell ref="A55:A60"/>
@@ -3645,12 +3644,13 @@
     <mergeCell ref="A97:A102"/>
     <mergeCell ref="A103:A108"/>
     <mergeCell ref="A109:A114"/>
-    <mergeCell ref="A43:A48"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A25:A30"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="A157:A162"/>
+    <mergeCell ref="A121:A126"/>
+    <mergeCell ref="A127:A132"/>
+    <mergeCell ref="A133:A138"/>
+    <mergeCell ref="A139:A144"/>
+    <mergeCell ref="A145:A150"/>
+    <mergeCell ref="A151:A156"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>